<commit_message>
更新样本。if getFileMd5(fpath) == readfile(os.path.join("tempdir", "xlsx", "result", fmd5)):
</commit_message>
<xml_diff>
--- a/kvision/ksample/mytable/BaiduOCRConverter_Excel/006_b1f38.xlsx
+++ b/kvision/ksample/mytable/BaiduOCRConverter_Excel/006_b1f38.xlsx
@@ -1,133 +1,45 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
-  <si>
-    <t>广东理工学院</t>
-  </si>
-  <si>
-    <t>肇庆学校</t>
-  </si>
-  <si>
-    <t>集团</t>
-  </si>
-  <si>
-    <t>可容纳学生人数</t>
-  </si>
-  <si>
-    <t>学校利用率</t>
-  </si>
-  <si>
-    <t>2015/2016</t>
-  </si>
-  <si>
-    <t>19,152</t>
-  </si>
-  <si>
-    <t>94.3%</t>
-  </si>
-  <si>
-    <t>6,829</t>
-  </si>
-  <si>
-    <t>87.6%</t>
-  </si>
-  <si>
-    <t>25,981</t>
-  </si>
-  <si>
-    <t>92.5%</t>
-  </si>
-  <si>
-    <t>2016/2017</t>
-  </si>
-  <si>
-    <t>90.1%</t>
-  </si>
-  <si>
-    <t>91.6%</t>
-  </si>
-  <si>
-    <t>90.5%</t>
-  </si>
-  <si>
-    <t>2017/2018</t>
-  </si>
-  <si>
-    <t>25.148</t>
-  </si>
-  <si>
-    <t>86.3%</t>
-  </si>
-  <si>
-    <t>81.3%</t>
-  </si>
-  <si>
-    <t>31,977</t>
-  </si>
-  <si>
-    <t>85.2%</t>
-  </si>
-  <si>
-    <t>2018/2019</t>
-  </si>
-  <si>
-    <t>29.148</t>
-  </si>
-  <si>
-    <t>90.8%</t>
-  </si>
-  <si>
-    <t>86.0%</t>
-  </si>
-  <si>
-    <t>35,977</t>
-  </si>
-  <si>
-    <t>89.9%</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="微软雅黑"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -135,21 +47,106 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color rgb="00FF0000"/>
+      </left>
+      <right style="thick">
+        <color rgb="00FF0000"/>
+      </right>
+      <top style="thick">
+        <color rgb="00FF0000"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="00FF0000"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -437,139 +434,219 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:7">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="G1" s="1"/>
+    <row r="1">
+      <c r="A1" s="2" t="n"/>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>广东理工学院</t>
+        </is>
+      </c>
+      <c r="C1" s="3" t="n"/>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>肇庆学校</t>
+        </is>
+      </c>
+      <c r="E1" s="3" t="n"/>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>集团</t>
+        </is>
+      </c>
+      <c r="G1" s="3" t="n"/>
     </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>4</v>
+    <row r="2">
+      <c r="A2" s="2" t="n"/>
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>可容纳学生人数</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="inlineStr">
+        <is>
+          <t>学校利用率</t>
+        </is>
+      </c>
+      <c r="D2" s="2" t="inlineStr">
+        <is>
+          <t>可容纳学生人数</t>
+        </is>
+      </c>
+      <c r="E2" s="2" t="inlineStr">
+        <is>
+          <t>学校利用率</t>
+        </is>
+      </c>
+      <c r="F2" s="2" t="inlineStr">
+        <is>
+          <t>可容纳学生人数</t>
+        </is>
+      </c>
+      <c r="G2" s="2" t="inlineStr">
+        <is>
+          <t>学校利用率</t>
+        </is>
       </c>
     </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>11</v>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>2015/2016</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="inlineStr">
+        <is>
+          <t>19,152</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="inlineStr">
+        <is>
+          <t>94.3%</t>
+        </is>
+      </c>
+      <c r="D3" s="2" t="inlineStr">
+        <is>
+          <t>6,829</t>
+        </is>
+      </c>
+      <c r="E3" s="2" t="inlineStr">
+        <is>
+          <t>87.6%</t>
+        </is>
+      </c>
+      <c r="F3" s="2" t="inlineStr">
+        <is>
+          <t>25,981</t>
+        </is>
+      </c>
+      <c r="G3" s="2" t="inlineStr">
+        <is>
+          <t>92.5%</t>
+        </is>
       </c>
     </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>15</v>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>2016/2017</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="inlineStr">
+        <is>
+          <t>19,152</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="inlineStr">
+        <is>
+          <t>90.1%</t>
+        </is>
+      </c>
+      <c r="D4" s="2" t="inlineStr">
+        <is>
+          <t>6,829</t>
+        </is>
+      </c>
+      <c r="E4" s="2" t="inlineStr">
+        <is>
+          <t>91.6%</t>
+        </is>
+      </c>
+      <c r="F4" s="2" t="inlineStr">
+        <is>
+          <t>25,981</t>
+        </is>
+      </c>
+      <c r="G4" s="2" t="inlineStr">
+        <is>
+          <t>90.5%</t>
+        </is>
       </c>
     </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>21</v>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>2017/2018</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>25.148</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="inlineStr">
+        <is>
+          <t>86.3%</t>
+        </is>
+      </c>
+      <c r="D5" s="2" t="inlineStr">
+        <is>
+          <t>6,829</t>
+        </is>
+      </c>
+      <c r="E5" s="2" t="inlineStr">
+        <is>
+          <t>81.3%</t>
+        </is>
+      </c>
+      <c r="F5" s="2" t="inlineStr">
+        <is>
+          <t>31,977</t>
+        </is>
+      </c>
+      <c r="G5" s="2" t="inlineStr">
+        <is>
+          <t>85.2%</t>
+        </is>
       </c>
     </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>27</v>
+    <row r="6">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>2018/2019</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="inlineStr">
+        <is>
+          <t>29.148</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="inlineStr">
+        <is>
+          <t>90.8%</t>
+        </is>
+      </c>
+      <c r="D6" s="2" t="inlineStr">
+        <is>
+          <t>6,829</t>
+        </is>
+      </c>
+      <c r="E6" s="2" t="inlineStr">
+        <is>
+          <t>86.0%</t>
+        </is>
+      </c>
+      <c r="F6" s="2" t="inlineStr">
+        <is>
+          <t>35,977</t>
+        </is>
+      </c>
+      <c r="G6" s="2" t="inlineStr">
+        <is>
+          <t>89.9%</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>